<commit_message>
noyon : changes : general app, hr app, support app added with its template
</commit_message>
<xml_diff>
--- a/assets/MenuList.xlsx
+++ b/assets/MenuList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\my-projects\ngohrms\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D05FA56-DC88-4239-9C08-251BEAFC59A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC09A2E-89A2-4044-90B9-C68C1FE8EE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Administration" sheetId="1" r:id="rId1"/>
@@ -875,11 +875,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="20.75" customWidth="1"/>
+    <col min="2" max="2" width="19.75" customWidth="1"/>
+    <col min="4" max="4" width="25.875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -972,7 +977,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F5" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F1 A5:C5 A2:C2 E2:F2 A3:C3 E3:F3 A4:C4 E4:F4 E5:F5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -981,7 +986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+    <sheetView topLeftCell="A134" workbookViewId="0">
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
noyon  : changes : hr portion added
</commit_message>
<xml_diff>
--- a/assets/MenuList.xlsx
+++ b/assets/MenuList.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\my-projects\ngohrms\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC09A2E-89A2-4044-90B9-C68C1FE8EE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97608365-D1DE-41B4-8048-B8611974CC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Administration" sheetId="1" r:id="rId1"/>
     <sheet name="HR" sheetId="3" r:id="rId2"/>
+    <sheet name="Fixed Asset" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="165">
   <si>
     <t>Menu Name</t>
   </si>
@@ -483,6 +484,39 @@
   </si>
   <si>
     <t>Sub-Section</t>
+  </si>
+  <si>
+    <t>Fixed Asset</t>
+  </si>
+  <si>
+    <t>/fixed-asset/</t>
+  </si>
+  <si>
+    <t>icons-Box-Open</t>
+  </si>
+  <si>
+    <t>Fixed Asset Import</t>
+  </si>
+  <si>
+    <t>/fixed-asset/import/</t>
+  </si>
+  <si>
+    <t>Maintenance Request</t>
+  </si>
+  <si>
+    <t>/fixed-asset/request-list/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maintenance Pending </t>
+  </si>
+  <si>
+    <t>/fixed-asset/maintenance-pending-list/</t>
+  </si>
+  <si>
+    <t>Vehicle Menagement</t>
+  </si>
+  <si>
+    <t>/vehicle-mangement/vehicle/</t>
   </si>
 </sst>
 </file>
@@ -525,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -534,6 +568,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,7 +912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2284,4 +2321,124 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5264EF73-180F-426D-B2D4-2878CECE1AF4}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Promotion/Demotion, Holyday setup, resgination
</commit_message>
<xml_diff>
--- a/assets/MenuList.xlsx
+++ b/assets/MenuList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Project\hrms\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A8341E-5406-430A-AFDD-071F40E5157E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34739E6B-0C29-4B25-9515-4C0D95F95FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="20568" windowHeight="10980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="20568" windowHeight="10980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Administration" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="169">
   <si>
     <t>Menu Name</t>
   </si>
@@ -523,6 +523,12 @@
   </si>
   <si>
     <t>Resignation</t>
+  </si>
+  <si>
+    <t>/hr/promotion-demotion/</t>
+  </si>
+  <si>
+    <t>Promotion/Demotion</t>
   </si>
 </sst>
 </file>
@@ -1027,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -2341,6 +2347,26 @@
       </c>
       <c r="F65" s="2">
         <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>168</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" t="s">
+        <v>116</v>
+      </c>
+      <c r="D66" t="s">
+        <v>167</v>
+      </c>
+      <c r="E66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66" s="2">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
noyon : employee branch transfer added
</commit_message>
<xml_diff>
--- a/assets/MenuList.xlsx
+++ b/assets/MenuList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Project\hrms\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\my-projects\ngohrms\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34739E6B-0C29-4B25-9515-4C0D95F95FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2DD4C1-E40A-4524-8A34-BF847422DF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="20568" windowHeight="10980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Administration" sheetId="1" r:id="rId1"/>
@@ -928,11 +928,11 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.69921875" customWidth="1"/>
-    <col min="2" max="2" width="19.69921875" customWidth="1"/>
-    <col min="4" max="4" width="25.8984375" customWidth="1"/>
+    <col min="1" max="1" width="20.75" customWidth="1"/>
+    <col min="2" max="2" width="19.75" customWidth="1"/>
+    <col min="4" max="4" width="25.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1035,15 +1035,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="10.69921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="2"/>
@@ -2383,7 +2383,7 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Entry date add in Resignation, Movement resgistry
</commit_message>
<xml_diff>
--- a/assets/MenuList.xlsx
+++ b/assets/MenuList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Project\hrms\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A604796-66D4-4220-A2E2-FBBFC8D98040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43A0236-BF38-435C-97F6-841AAF8BC1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="1260" windowWidth="20568" windowHeight="10980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2472" yWindow="1260" windowWidth="20568" windowHeight="10980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Administration" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="161">
   <si>
     <t>Menu Name</t>
   </si>
@@ -499,6 +499,12 @@
   </si>
   <si>
     <t>/fixed-asset/</t>
+  </si>
+  <si>
+    <t>/hr/movement-registry/</t>
+  </si>
+  <si>
+    <t>Movement Registry</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -2316,6 +2322,26 @@
         <v>26</v>
       </c>
     </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>160</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" t="s">
+        <v>116</v>
+      </c>
+      <c r="D66" t="s">
+        <v>159</v>
+      </c>
+      <c r="E66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66" s="2">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2326,7 +2352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B919484B-B9D3-472D-B474-503D21D2FB40}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>